<commit_message>
Adding year in ExploreData and Parametres Fixing typos in lgtm.py Fixing amounts
</commit_message>
<xml_diff>
--- a/src/france/data/sources/IRPP_PPE.xlsx
+++ b/src/france/data/sources/IRPP_PPE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>ppe nb FF non imposables</t>
   </si>
@@ -156,16 +156,10 @@
     <t>FRANCE ENTIERE (DGFP)</t>
   </si>
   <si>
-    <t xml:space="preserve">ces données sont issues du même tableau Insee comptes nationaux, le problème c'est que le montant de l'irpp ne correspond pas aux données au dessus, mais si nous prenons ces données là pour la csg et la crds nous devrions peut-être prendre aussi celles pour l'irpp… qu'en penses-tu ? </t>
-  </si>
-  <si>
     <t>irpp</t>
   </si>
   <si>
     <t>ppe</t>
-  </si>
-  <si>
-    <t>J'ai pris les données insee également pour l'irpp</t>
   </si>
   <si>
     <t>var</t>
@@ -348,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -873,54 +867,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -985,7 +931,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1149,7 +1095,6 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1162,26 +1107,16 @@
     <xf numFmtId="164" fontId="9" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1191,7 +1126,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1199,56 +1134,48 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1557,20 +1484,20 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="136">
+      <c r="A1" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="138">
         <v>2002</v>
       </c>
       <c r="C1" s="137">
@@ -1599,68 +1526,86 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="136" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="130"/>
+      <c r="C2" s="131">
+        <v>17582623</v>
+      </c>
+      <c r="D2" s="131">
+        <v>17922453</v>
+      </c>
+      <c r="E2" s="131">
+        <v>18635634</v>
+      </c>
+      <c r="F2" s="131">
+        <v>18833659</v>
+      </c>
+      <c r="G2" s="131">
+        <v>19440573</v>
+      </c>
+      <c r="H2" s="131">
+        <v>19176732</v>
+      </c>
+      <c r="I2" s="131">
+        <v>19316055</v>
+      </c>
+      <c r="J2" s="131"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="139">
-        <v>17582623</v>
-      </c>
-      <c r="D2" s="139">
-        <v>17922453</v>
-      </c>
-      <c r="E2" s="139">
-        <v>18635634</v>
-      </c>
-      <c r="F2" s="139">
-        <v>18833659</v>
-      </c>
-      <c r="G2" s="139">
-        <v>19440573</v>
-      </c>
-      <c r="H2" s="139">
-        <v>19176732</v>
-      </c>
-      <c r="I2" s="139">
-        <v>19316055</v>
-      </c>
-      <c r="J2" s="140"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="141"/>
-      <c r="C3" s="139">
+      <c r="B3" s="132"/>
+      <c r="C3" s="131">
         <v>8482456</v>
       </c>
-      <c r="D3" s="139">
+      <c r="D3" s="131">
         <v>8909421</v>
       </c>
-      <c r="E3" s="139">
+      <c r="E3" s="131">
         <v>8380886</v>
       </c>
-      <c r="F3" s="139">
+      <c r="F3" s="131">
         <v>8715310</v>
       </c>
-      <c r="G3" s="139">
+      <c r="G3" s="131">
         <v>8686706</v>
       </c>
-      <c r="H3" s="139">
+      <c r="H3" s="131">
         <v>7984054</v>
       </c>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="135" t="s">
-        <v>50</v>
-      </c>
+      <c r="A4" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="146" t="s">
+      <c r="A5" s="136" t="s">
         <v>17</v>
       </c>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1673,11 +1618,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="5" width="12.7109375" customWidth="1"/>
@@ -1689,161 +1635,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="142">
+      <c r="A1" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="141">
         <v>2002</v>
       </c>
-      <c r="C1" s="143">
+      <c r="C1" s="142">
         <v>2003</v>
       </c>
-      <c r="D1" s="143">
+      <c r="D1" s="142">
         <v>2004</v>
       </c>
-      <c r="E1" s="143">
+      <c r="E1" s="142">
         <v>2005</v>
       </c>
-      <c r="F1" s="143">
+      <c r="F1" s="142">
         <v>2006</v>
       </c>
-      <c r="G1" s="143">
+      <c r="G1" s="142">
         <v>2007</v>
       </c>
-      <c r="H1" s="143">
+      <c r="H1" s="142">
         <v>2008</v>
       </c>
-      <c r="I1" s="143">
+      <c r="I1" s="142">
         <v>2009</v>
       </c>
-      <c r="J1" s="143">
+      <c r="J1" s="142">
         <v>2010</v>
       </c>
-      <c r="K1" s="135"/>
+      <c r="K1" s="136">
+        <v>2011</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="136" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="134">
+        <v>47300000000</v>
+      </c>
+      <c r="C2" s="134">
+        <v>47600000000</v>
+      </c>
+      <c r="D2" s="134">
+        <v>49400000000</v>
+      </c>
+      <c r="E2" s="134">
+        <v>52400000000</v>
+      </c>
+      <c r="F2" s="134">
+        <v>48600000000</v>
+      </c>
+      <c r="G2" s="134">
+        <v>50900000000</v>
+      </c>
+      <c r="H2" s="134">
+        <v>46100000000</v>
+      </c>
+      <c r="I2" s="134">
+        <v>47000000000</v>
+      </c>
+      <c r="J2" s="134">
+        <v>50600000000</v>
+      </c>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="148">
-        <v>47300000000</v>
-      </c>
-      <c r="D2" s="148">
-        <v>47600000000</v>
-      </c>
-      <c r="E2" s="148">
-        <v>49400000000</v>
-      </c>
-      <c r="F2" s="148">
-        <v>52400000000</v>
-      </c>
-      <c r="G2" s="148">
-        <v>48600000000</v>
-      </c>
-      <c r="H2" s="148">
-        <v>50900000000</v>
-      </c>
-      <c r="I2" s="148">
-        <v>46100000000</v>
-      </c>
-      <c r="J2" s="148">
-        <v>47000000000</v>
-      </c>
-      <c r="K2" s="149">
-        <v>50600000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="141"/>
-      <c r="C3" s="148">
+      <c r="B3" s="132"/>
+      <c r="C3" s="134">
         <v>2374667371</v>
       </c>
-      <c r="D3" s="148">
+      <c r="D3" s="134">
         <v>2610279209</v>
       </c>
-      <c r="E3" s="148">
+      <c r="E3" s="134">
         <v>3143226143</v>
       </c>
-      <c r="F3" s="148">
+      <c r="F3" s="134">
         <v>4393772272</v>
       </c>
-      <c r="G3" s="148">
+      <c r="G3" s="134">
         <v>4353215945</v>
       </c>
-      <c r="H3" s="148">
+      <c r="H3" s="134">
         <v>3793069273</v>
       </c>
-      <c r="I3" s="150"/>
-      <c r="J3" s="151"/>
-      <c r="K3" s="152"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="144" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="148">
+      <c r="A4" s="140" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="139"/>
+      <c r="C4" s="134">
         <v>64100000000</v>
       </c>
-      <c r="D4" s="148">
+      <c r="D4" s="134">
         <v>66000000000</v>
       </c>
-      <c r="E4" s="148">
+      <c r="E4" s="134">
         <v>70800000000</v>
       </c>
-      <c r="F4" s="148">
+      <c r="F4" s="134">
         <v>75500000000</v>
       </c>
-      <c r="G4" s="148">
+      <c r="G4" s="134">
         <v>79200000000</v>
       </c>
-      <c r="H4" s="148">
+      <c r="H4" s="134">
         <v>83400000000</v>
       </c>
-      <c r="I4" s="148">
+      <c r="I4" s="134">
         <v>80800000000</v>
       </c>
-      <c r="J4" s="148">
+      <c r="J4" s="134">
         <v>82300000000</v>
       </c>
-      <c r="K4" s="149">
+      <c r="K4" s="134">
         <v>87400000000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="148">
+      <c r="B5" s="139"/>
+      <c r="C5" s="134">
         <v>4800000000</v>
       </c>
-      <c r="D5" s="148">
+      <c r="D5" s="134">
         <v>5000000000</v>
       </c>
-      <c r="E5" s="148">
+      <c r="E5" s="134">
         <v>4900000000</v>
       </c>
-      <c r="F5" s="148">
+      <c r="F5" s="134">
         <v>5500000000</v>
       </c>
-      <c r="G5" s="148">
+      <c r="G5" s="134">
         <v>5800000000</v>
       </c>
-      <c r="H5" s="148">
+      <c r="H5" s="134">
         <v>6100000000</v>
       </c>
-      <c r="I5" s="148">
+      <c r="I5" s="134">
         <v>6000000000</v>
       </c>
-      <c r="J5" s="148">
+      <c r="J5" s="134">
         <v>6000000000</v>
       </c>
-      <c r="K5" s="149">
+      <c r="K5" s="134">
         <v>6300000000</v>
       </c>
     </row>
@@ -1950,7 +1898,7 @@
       <c r="J2" s="8">
         <v>2010</v>
       </c>
-      <c r="K2" s="134"/>
+      <c r="K2" s="129"/>
       <c r="L2" s="91"/>
       <c r="M2" s="91"/>
       <c r="N2" s="91"/>
@@ -4401,8 +4349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4416,34 +4364,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="110">
+      <c r="B1" s="109">
         <v>2002</v>
       </c>
-      <c r="C1" s="110">
+      <c r="C1" s="109">
         <v>2003</v>
       </c>
-      <c r="D1" s="110">
+      <c r="D1" s="109">
         <v>2004</v>
       </c>
-      <c r="E1" s="110">
+      <c r="E1" s="109">
         <v>2005</v>
       </c>
-      <c r="F1" s="110">
+      <c r="F1" s="109">
         <v>2006</v>
       </c>
-      <c r="G1" s="110">
+      <c r="G1" s="109">
         <v>2007</v>
       </c>
-      <c r="H1" s="110">
+      <c r="H1" s="109">
         <v>2008</v>
       </c>
-      <c r="I1" s="110">
+      <c r="I1" s="109">
         <v>2009</v>
       </c>
-      <c r="J1" s="116">
+      <c r="J1" s="111">
         <v>2010</v>
       </c>
-      <c r="K1" s="127">
+      <c r="K1" s="122">
         <v>2011</v>
       </c>
     </row>
@@ -4476,7 +4424,7 @@
       <c r="J2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="128"/>
+      <c r="K2" s="123"/>
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4491,7 +4439,7 @@
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
-      <c r="J3" s="117"/>
+      <c r="J3" s="112"/>
       <c r="K3" s="74"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4506,8 +4454,8 @@
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="126"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="121"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
@@ -4535,7 +4483,7 @@
       <c r="I5" s="32">
         <v>45006902661</v>
       </c>
-      <c r="J5" s="119"/>
+      <c r="J5" s="114"/>
       <c r="K5" s="74"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4568,7 +4516,7 @@
         <v>53607000000</v>
       </c>
       <c r="I6" s="32"/>
-      <c r="J6" s="119"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="74"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4595,8 +4543,8 @@
         <v>3793069273</v>
       </c>
       <c r="I7" s="27"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="125"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="120"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
@@ -4622,7 +4570,7 @@
         <v>1533120926</v>
       </c>
       <c r="I8" s="27"/>
-      <c r="J8" s="120"/>
+      <c r="J8" s="115"/>
       <c r="K8" s="74"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4649,7 +4597,7 @@
         <v>2259948347</v>
       </c>
       <c r="I9" s="53"/>
-      <c r="J9" s="121"/>
+      <c r="J9" s="116"/>
       <c r="K9" s="74"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4664,7 +4612,7 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
-      <c r="J10" s="122"/>
+      <c r="J10" s="117"/>
       <c r="K10" s="74"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4693,7 +4641,7 @@
         <v>48435000000</v>
       </c>
       <c r="I11" s="69"/>
-      <c r="J11" s="123"/>
+      <c r="J11" s="118"/>
       <c r="K11" s="74"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4722,7 +4670,7 @@
       <c r="I12" s="55">
         <v>45469619577</v>
       </c>
-      <c r="J12" s="124"/>
+      <c r="J12" s="119"/>
       <c r="K12" s="74"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4751,7 +4699,7 @@
         <v>54292000000</v>
       </c>
       <c r="I13" s="55"/>
-      <c r="J13" s="124"/>
+      <c r="J13" s="119"/>
       <c r="K13" s="74"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4778,7 +4726,7 @@
         <v>3917700000</v>
       </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="120"/>
+      <c r="J14" s="115"/>
       <c r="K14" s="74"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4805,78 +4753,76 @@
         <v>1553200000</v>
       </c>
       <c r="I15" s="27"/>
-      <c r="J15" s="120"/>
+      <c r="J15" s="115"/>
       <c r="K15" s="74"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="124" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="17"/>
-      <c r="C16" s="130">
+      <c r="C16" s="125">
         <v>1498600000</v>
       </c>
-      <c r="D16" s="130">
+      <c r="D16" s="125">
         <v>1597200000</v>
       </c>
-      <c r="E16" s="130">
+      <c r="E16" s="125">
         <v>1854500000</v>
       </c>
-      <c r="F16" s="130">
+      <c r="F16" s="125">
         <v>2536900000</v>
       </c>
-      <c r="G16" s="130">
+      <c r="G16" s="125">
         <v>2514800000</v>
       </c>
-      <c r="H16" s="131">
+      <c r="H16" s="126">
         <v>2364500000</v>
       </c>
-      <c r="I16" s="132"/>
-      <c r="J16" s="133"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="128"/>
       <c r="K16" s="17"/>
       <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="108">
+      <c r="B17" s="144"/>
+      <c r="C17" s="107">
         <v>2003</v>
       </c>
-      <c r="D17" s="108">
+      <c r="D17" s="107">
         <v>2004</v>
       </c>
-      <c r="E17" s="108">
+      <c r="E17" s="107">
         <v>2005</v>
       </c>
-      <c r="F17" s="108">
+      <c r="F17" s="107">
         <v>2006</v>
       </c>
-      <c r="G17" s="108">
+      <c r="G17" s="107">
         <v>2007</v>
       </c>
-      <c r="H17" s="108">
+      <c r="H17" s="107">
         <v>2008</v>
       </c>
-      <c r="I17" s="108">
+      <c r="I17" s="107">
         <v>2009</v>
       </c>
-      <c r="J17" s="108">
+      <c r="J17" s="107">
         <v>2010</v>
       </c>
-      <c r="K17" s="109">
+      <c r="K17" s="108">
         <v>2011</v>
       </c>
-      <c r="L17" s="154" t="s">
-        <v>45</v>
-      </c>
+      <c r="L17" s="147"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="113"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="72">
         <v>64100000000</v>
       </c>
@@ -4904,13 +4850,13 @@
       <c r="K18" s="105">
         <v>87400000000</v>
       </c>
-      <c r="L18" s="154"/>
+      <c r="L18" s="147"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="113"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="72">
         <v>4800000000</v>
       </c>
@@ -4938,80 +4884,78 @@
       <c r="K19" s="105">
         <v>6300000000</v>
       </c>
-      <c r="L19" s="154"/>
+      <c r="L19" s="147"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="114"/>
+      <c r="B20" s="72">
+        <v>47300000000</v>
+      </c>
       <c r="C20" s="72">
-        <v>47300000000</v>
+        <v>47600000000</v>
       </c>
       <c r="D20" s="72">
-        <v>47600000000</v>
+        <v>49400000000</v>
       </c>
       <c r="E20" s="72">
-        <v>49400000000</v>
+        <v>52400000000</v>
       </c>
       <c r="F20" s="72">
-        <v>52400000000</v>
+        <v>48600000000</v>
       </c>
       <c r="G20" s="72">
-        <v>48600000000</v>
+        <v>50900000000</v>
       </c>
       <c r="H20" s="72">
-        <v>50900000000</v>
+        <v>46100000000</v>
       </c>
       <c r="I20" s="72">
-        <v>46100000000</v>
+        <v>47000000000</v>
       </c>
       <c r="J20" s="72">
-        <v>47000000000</v>
-      </c>
-      <c r="K20" s="105">
         <v>50600000000</v>
       </c>
-      <c r="L20" s="154"/>
+      <c r="K20" s="145"/>
+      <c r="L20" s="147"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="115"/>
+      <c r="B21" s="106">
+        <v>36100000000</v>
+      </c>
       <c r="C21" s="106">
-        <v>36100000000</v>
+        <v>40800000000</v>
       </c>
       <c r="D21" s="106">
-        <v>40800000000</v>
+        <v>41800000000</v>
       </c>
       <c r="E21" s="106">
-        <v>41800000000</v>
+        <v>48400000000</v>
       </c>
       <c r="F21" s="106">
-        <v>48400000000</v>
+        <v>51400000000</v>
       </c>
       <c r="G21" s="106">
-        <v>51400000000</v>
+        <v>49500000000</v>
       </c>
       <c r="H21" s="106">
-        <v>49500000000</v>
+        <v>20900000000</v>
       </c>
       <c r="I21" s="106">
-        <v>20900000000</v>
+        <v>33100000000</v>
       </c>
       <c r="J21" s="106">
-        <v>33100000000</v>
-      </c>
-      <c r="K21" s="107">
         <v>41900000000</v>
       </c>
-      <c r="L21" s="154"/>
+      <c r="K21" s="146"/>
+      <c r="L21" s="147"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L22" s="145" t="s">
-        <v>48</v>
-      </c>
+      <c r="L22" s="133"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>

</xml_diff>